<commit_message>
update with conditional formating and check for error
</commit_message>
<xml_diff>
--- a/Score Sheet/Rocking_Rover-Score_Sheet.xlsx
+++ b/Score Sheet/Rocking_Rover-Score_Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdongol/RockingRover/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdongol/RockingRover/Score Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2255381B-1F29-FF49-86A5-0FB58E91761A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C0CCD-519A-A84A-91AA-D142E918302E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{5677EDF9-9A5E-3B4C-B208-F3D76B1A2241}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="107">
   <si>
     <t>Mission</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>10 each circle</t>
+  </si>
+  <si>
+    <t>No# of Complete Circle</t>
   </si>
 </sst>
 </file>
@@ -791,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -906,36 +909,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -944,11 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -960,73 +934,14 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1049,13 +964,31 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1064,33 +997,100 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="62">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="67">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1123,6 +1123,56 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1138,6 +1188,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1761,7 +1821,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$L$37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$L$37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1878,6 +1938,10 @@
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="15" fmlaLink="$K$69" fmlaRange="Sheet2!$C$2:$D$8" noThreeD="1" sel="7" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="15" fmlaLink="K67" fmlaRange="Sheet2!$B$2:$B$7" noThreeD="1" sel="6" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6038,6 +6102,64 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>25400</xdr:colOff>
+          <xdr:row>66</xdr:row>
+          <xdr:rowOff>12700</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>11</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>66</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1101" name="Drop Down 77" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1101"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D876C043-FB5F-BD4C-ADC4-4ABA23F83198}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -6344,8 +6466,8 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M63" sqref="M63"/>
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K73" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6365,28 +6487,28 @@
       <c r="A1" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="88" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="89">
+      <c r="M1" s="59"/>
+      <c r="N1" s="60">
         <f>IF(OR(N69="NA",N63="NA",N55="NA",N52="NA",N48="NA",N43="NA",N40="NA",N37="NA",N34="NA",N30="NA",N27="NA",N24="NA",N22="NA",N18="NA",N15="NA",N12="NA",N8="NA",N6="NA"),"NA",SUM(N69,N63,N55,N52,N48,N43,N40,N37,N34,N30,N27,N24,N22,N18,N15,N12,N8,N6))</f>
-        <v>720</v>
-      </c>
-      <c r="O1" s="90" t="str">
-        <f>IF(N1=720,"🌟","")</f>
+        <v>740</v>
+      </c>
+      <c r="O1" s="61" t="str">
+        <f>IF(N1=740,"🌟","")</f>
         <v>🌟</v>
       </c>
     </row>
@@ -6394,22 +6516,22 @@
       <c r="A2" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="92">
+      <c r="B2" s="65">
         <v>52520</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="90"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="61"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
@@ -6429,61 +6551,61 @@
       <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="64" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="65"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="55"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="58"/>
-      <c r="B6" s="56" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="90" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
       <c r="K6" s="25"/>
       <c r="L6" s="12" t="b">
         <v>1</v>
@@ -6497,123 +6619,123 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="55"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="62" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="50" t="s">
+      <c r="G8" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="51" t="b">
+      <c r="L8" s="96" t="b">
         <v>1</v>
       </c>
-      <c r="M8" s="66">
+      <c r="M8" s="76">
         <v>20</v>
       </c>
-      <c r="N8" s="46">
+      <c r="N8" s="83">
         <f>IF(L8=TRUE,M8,"")</f>
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="46"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="83"/>
     </row>
     <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="61"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="27"/>
-      <c r="L10" s="52"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="47"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="77"/>
+      <c r="N10" s="84"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="55"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="68"/>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="50" t="s">
+      <c r="G12" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="26"/>
       <c r="L12" s="16" t="b">
         <v>0</v>
@@ -6621,24 +6743,24 @@
       <c r="M12" s="2">
         <v>20</v>
       </c>
-      <c r="N12" s="46">
+      <c r="N12" s="83">
         <f>IF(AND(L12,L13)=TRUE,"NA",IF(L12=TRUE,M12,IF(L13=TRUE,M13,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="58"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="53" t="s">
+      <c r="G13" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="26"/>
       <c r="L13" s="16" t="b">
         <v>1</v>
@@ -6646,41 +6768,41 @@
       <c r="M13" s="3">
         <v>30</v>
       </c>
-      <c r="N13" s="47"/>
+      <c r="N13" s="84"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="76" t="s">
+      <c r="B14" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="77"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="89"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="74" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="75"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
       <c r="K15" s="28"/>
       <c r="L15" s="16" t="b">
         <v>1</v>
@@ -6688,24 +6810,24 @@
       <c r="M15" s="2">
         <v>20</v>
       </c>
-      <c r="N15" s="46">
+      <c r="N15" s="83">
         <f>IF(AND(L15,L16)=TRUE,M15+M16,IF(L15=TRUE,M15,IF(L16=TRUE,M16,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="61"/>
-      <c r="B16" s="53" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="26"/>
       <c r="L16" s="16" t="b">
         <v>1</v>
@@ -6713,41 +6835,41 @@
       <c r="M16" s="3">
         <v>10</v>
       </c>
-      <c r="N16" s="47"/>
+      <c r="N16" s="84"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="54" t="s">
+      <c r="B17" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="55"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="68"/>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="72"/>
-      <c r="H18" s="72"/>
-      <c r="I18" s="72"/>
-      <c r="J18" s="72"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
       <c r="K18" s="29"/>
       <c r="L18" s="16" t="b">
         <v>1</v>
@@ -6762,17 +6884,17 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="68"/>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
       <c r="K19" s="26"/>
       <c r="L19" s="16" t="b">
         <v>1</v>
@@ -6783,18 +6905,18 @@
       <c r="N19" s="48"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="58"/>
-      <c r="B20" s="53" t="s">
+      <c r="A20" s="69"/>
+      <c r="B20" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="26"/>
       <c r="L20" s="16" t="b">
         <v>1</v>
@@ -6802,41 +6924,41 @@
       <c r="M20" s="3">
         <v>10</v>
       </c>
-      <c r="N20" s="49"/>
+      <c r="N20" s="70"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="54" t="s">
+      <c r="B21" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="55"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="61"/>
-      <c r="B22" s="73" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="95"/>
+      <c r="G22" s="95"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="95"/>
+      <c r="J22" s="95"/>
       <c r="K22" s="4"/>
       <c r="L22" s="16" t="b">
         <v>1</v>
@@ -6850,35 +6972,35 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="57" t="s">
+      <c r="A23" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
-      <c r="M23" s="54"/>
-      <c r="N23" s="55"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="68"/>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
       <c r="H24" s="23"/>
       <c r="I24" s="30" t="s">
         <v>87</v>
@@ -6891,19 +7013,19 @@
       <c r="M24" s="2">
         <v>20</v>
       </c>
-      <c r="N24" s="46">
+      <c r="N24" s="83">
         <f>IF(AND(L24,L25)=TRUE,"NA",IF(L24=TRUE,M24,IF(L25=TRUE,M25,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="58"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
+      <c r="A25" s="69"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
       <c r="H25" s="23"/>
       <c r="I25" s="25" t="s">
         <v>88</v>
@@ -6916,41 +7038,41 @@
       <c r="M25" s="3">
         <v>30</v>
       </c>
-      <c r="N25" s="47"/>
+      <c r="N25" s="84"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="59" t="s">
+      <c r="A26" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
-      <c r="M26" s="54"/>
-      <c r="N26" s="55"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="60"/>
-      <c r="B27" s="50" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="50"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
       <c r="K27" s="26"/>
       <c r="L27" s="16" t="b">
         <v>1</v>
@@ -6958,24 +7080,24 @@
       <c r="M27" s="6">
         <v>20</v>
       </c>
-      <c r="N27" s="46">
+      <c r="N27" s="83">
         <f>IF(IF(L27=TRUE,M27,0)+IF(L28=TRUE,M28,0)=0, "", IF(L27=TRUE,M27,0)+IF(L28=TRUE,M28,0))</f>
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="61"/>
-      <c r="B28" s="53" t="s">
+      <c r="A28" s="51"/>
+      <c r="B28" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
       <c r="K28" s="26"/>
       <c r="L28" s="16" t="b">
         <v>1</v>
@@ -6983,41 +7105,41 @@
       <c r="M28" s="7">
         <v>10</v>
       </c>
-      <c r="N28" s="47"/>
+      <c r="N28" s="84"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="54"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="54"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="55"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="68"/>
-      <c r="B30" s="50" t="s">
+      <c r="B30" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
       <c r="K30" s="26"/>
       <c r="L30" s="16" t="b">
         <v>1</v>
@@ -7032,17 +7154,17 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="68"/>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
       <c r="K31" s="26"/>
       <c r="L31" s="16" t="b">
         <v>1</v>
@@ -7053,18 +7175,18 @@
       <c r="N31" s="48"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="58"/>
-      <c r="B32" s="53" t="s">
+      <c r="A32" s="69"/>
+      <c r="B32" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
       <c r="K32" s="26"/>
       <c r="L32" s="16" t="b">
         <v>1</v>
@@ -7072,41 +7194,41 @@
       <c r="M32" s="7">
         <v>10</v>
       </c>
-      <c r="N32" s="49"/>
+      <c r="N32" s="70"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="54" t="s">
+      <c r="B33" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="54"/>
-      <c r="M33" s="54"/>
-      <c r="N33" s="55"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="47"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="60"/>
-      <c r="B34" s="50" t="s">
+      <c r="A34" s="50"/>
+      <c r="B34" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="26"/>
       <c r="L34" s="16" t="b">
         <v>1</v>
@@ -7114,24 +7236,24 @@
       <c r="M34" s="6">
         <v>20</v>
       </c>
-      <c r="N34" s="46">
+      <c r="N34" s="83">
         <f>IF(AND(L34,L35)=TRUE,M34+M35,IF(L34=TRUE,M34,IF(L35=TRUE,M35,"")))</f>
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="61"/>
-      <c r="B35" s="53" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
       <c r="K35" s="26"/>
       <c r="L35" s="16" t="b">
         <v>1</v>
@@ -7139,104 +7261,104 @@
       <c r="M35" s="7">
         <v>20</v>
       </c>
-      <c r="N35" s="47"/>
+      <c r="N35" s="84"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="55"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="47"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="68"/>
-      <c r="B37" s="69" t="s">
+      <c r="B37" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="69"/>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
-      <c r="F37" s="69"/>
-      <c r="G37" s="69"/>
-      <c r="H37" s="69"/>
-      <c r="I37" s="69"/>
-      <c r="J37" s="69"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
       <c r="K37" s="31"/>
       <c r="L37" s="78" t="b">
-        <v>0</v>
-      </c>
-      <c r="M37" s="66">
+        <v>1</v>
+      </c>
+      <c r="M37" s="76">
         <v>20</v>
       </c>
-      <c r="N37" s="48" t="str">
+      <c r="N37" s="48">
         <f t="shared" ref="N37" si="0">IF(L37=TRUE,M37,"")</f>
-        <v/>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="58"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
       <c r="K38" s="32"/>
       <c r="L38" s="79"/>
-      <c r="M38" s="67"/>
-      <c r="N38" s="49"/>
+      <c r="M38" s="77"/>
+      <c r="N38" s="70"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="59" t="s">
+      <c r="A39" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="54"/>
-      <c r="L39" s="54"/>
-      <c r="M39" s="54"/>
-      <c r="N39" s="55"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="60"/>
-      <c r="B40" s="44" t="s">
+      <c r="A40" s="50"/>
+      <c r="B40" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="50" t="s">
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="J40" s="50"/>
+      <c r="J40" s="45"/>
       <c r="K40" s="26"/>
       <c r="L40" s="16" t="b">
         <v>0</v>
@@ -7244,24 +7366,24 @@
       <c r="M40" s="2">
         <v>20</v>
       </c>
-      <c r="N40" s="46">
+      <c r="N40" s="83">
         <f>IF(AND(L40,L41)=TRUE,"NA",IF(L40=TRUE,M40,IF(L41=TRUE,M41,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="61"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="53" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="74"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="J41" s="53"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="26"/>
       <c r="L41" s="16" t="b">
         <v>1</v>
@@ -7269,43 +7391,43 @@
       <c r="M41" s="3">
         <v>30</v>
       </c>
-      <c r="N41" s="47"/>
+      <c r="N41" s="84"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="96"/>
-      <c r="D42" s="96"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="96"/>
-      <c r="I42" s="96"/>
-      <c r="J42" s="96"/>
-      <c r="K42" s="96"/>
-      <c r="L42" s="96"/>
-      <c r="M42" s="96"/>
-      <c r="N42" s="97"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="53"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="68"/>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="50" t="s">
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="J43" s="50"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="26"/>
       <c r="L43" s="16" t="b">
         <v>0</v>
@@ -7320,17 +7442,17 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="68"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44"/>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="50" t="s">
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="J44" s="50"/>
+      <c r="J44" s="45"/>
       <c r="K44" s="26"/>
       <c r="L44" s="16" t="b">
         <v>1</v>
@@ -7342,19 +7464,19 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="68"/>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="50" t="s">
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="73"/>
+      <c r="I45" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="J45" s="50"/>
+      <c r="J45" s="45"/>
       <c r="K45" s="26"/>
       <c r="L45" s="16" t="b">
         <v>0</v>
@@ -7365,18 +7487,18 @@
       <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="58"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="53" t="s">
+      <c r="A46" s="69"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
+      <c r="E46" s="74"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="74"/>
+      <c r="I46" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="J46" s="53"/>
+      <c r="J46" s="54"/>
       <c r="K46" s="26"/>
       <c r="L46" s="16" t="b">
         <v>1</v>
@@ -7384,41 +7506,41 @@
       <c r="M46" s="3">
         <v>10</v>
       </c>
-      <c r="N46" s="49"/>
+      <c r="N46" s="70"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="55"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="47"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="60"/>
-      <c r="B48" s="50" t="s">
+      <c r="A48" s="50"/>
+      <c r="B48" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
       <c r="K48" s="26"/>
       <c r="L48" s="16" t="b">
         <v>1</v>
@@ -7432,18 +7554,18 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="60"/>
-      <c r="B49" s="50" t="s">
+      <c r="A49" s="50"/>
+      <c r="B49" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
       <c r="K49" s="26"/>
       <c r="L49" s="16" t="b">
         <v>1</v>
@@ -7454,18 +7576,18 @@
       <c r="N49" s="48"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="61"/>
-      <c r="B50" s="53" t="s">
+      <c r="A50" s="51"/>
+      <c r="B50" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
       <c r="K50" s="26"/>
       <c r="L50" s="16" t="b">
         <v>1</v>
@@ -7473,43 +7595,43 @@
       <c r="M50" s="3">
         <v>10</v>
       </c>
-      <c r="N50" s="49"/>
+      <c r="N50" s="70"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="57" t="s">
+      <c r="A51" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C51" s="54"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="54"/>
-      <c r="M51" s="54"/>
-      <c r="N51" s="55"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="47"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="68"/>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44" t="s">
+      <c r="C52" s="73"/>
+      <c r="D52" s="73"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="J52" s="44"/>
+      <c r="J52" s="73"/>
       <c r="K52" s="33"/>
       <c r="L52" s="16" t="b">
         <v>1</v>
@@ -7517,22 +7639,22 @@
       <c r="M52" s="2">
         <v>10</v>
       </c>
-      <c r="N52" s="46">
+      <c r="N52" s="83">
         <f>IF(AND(L52,L53)=TRUE,M52+M53,IF(L52=TRUE,M52,IF(L53=TRUE,M53,"")))</f>
         <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="58"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="45"/>
-      <c r="J53" s="45"/>
+      <c r="A53" s="69"/>
+      <c r="B53" s="74"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
+      <c r="F53" s="74"/>
+      <c r="G53" s="74"/>
+      <c r="H53" s="74"/>
+      <c r="I53" s="74"/>
+      <c r="J53" s="74"/>
       <c r="K53" s="33"/>
       <c r="L53" s="16" t="b">
         <v>1</v>
@@ -7540,43 +7662,43 @@
       <c r="M53" s="2">
         <v>10</v>
       </c>
-      <c r="N53" s="47"/>
+      <c r="N53" s="84"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="59" t="s">
+      <c r="A54" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="54"/>
-      <c r="J54" s="54"/>
-      <c r="K54" s="54"/>
-      <c r="L54" s="54"/>
-      <c r="M54" s="54"/>
-      <c r="N54" s="55"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46"/>
+      <c r="N54" s="47"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="60"/>
-      <c r="B55" s="44" t="s">
+      <c r="A55" s="50"/>
+      <c r="B55" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="44"/>
-      <c r="E55" s="44"/>
-      <c r="F55" s="44"/>
-      <c r="G55" s="44"/>
-      <c r="H55" s="44" t="s">
+      <c r="C55" s="73"/>
+      <c r="D55" s="73"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="I55" s="44"/>
-      <c r="J55" s="83" t="s">
+      <c r="I55" s="73"/>
+      <c r="J55" s="85" t="s">
         <v>56</v>
       </c>
       <c r="K55" s="34"/>
@@ -7592,16 +7714,16 @@
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="60"/>
-      <c r="B56" s="44"/>
-      <c r="C56" s="44"/>
-      <c r="D56" s="44"/>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="44"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="44"/>
-      <c r="J56" s="83"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="73"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
+      <c r="I56" s="73"/>
+      <c r="J56" s="85"/>
       <c r="K56" s="34"/>
       <c r="L56" s="17" t="b">
         <v>1</v>
@@ -7612,18 +7734,18 @@
       <c r="N56" s="48"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="60"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44" t="s">
+      <c r="A57" s="50"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="73"/>
+      <c r="G57" s="73"/>
+      <c r="H57" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="I57" s="44"/>
-      <c r="J57" s="83" t="s">
+      <c r="I57" s="73"/>
+      <c r="J57" s="85" t="s">
         <v>60</v>
       </c>
       <c r="K57" s="34"/>
@@ -7636,16 +7758,16 @@
       <c r="N57" s="48"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="60"/>
-      <c r="B58" s="44"/>
-      <c r="C58" s="44"/>
-      <c r="D58" s="44"/>
-      <c r="E58" s="44"/>
-      <c r="F58" s="44"/>
-      <c r="G58" s="44"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="44"/>
-      <c r="J58" s="83"/>
+      <c r="A58" s="50"/>
+      <c r="B58" s="73"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
+      <c r="G58" s="73"/>
+      <c r="H58" s="73"/>
+      <c r="I58" s="73"/>
+      <c r="J58" s="85"/>
       <c r="K58" s="34"/>
       <c r="L58" s="16" t="b">
         <v>1</v>
@@ -7656,18 +7778,18 @@
       <c r="N58" s="48"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="60"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="44"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44" t="s">
+      <c r="A59" s="50"/>
+      <c r="B59" s="73"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="I59" s="44"/>
-      <c r="J59" s="83" t="s">
+      <c r="I59" s="73"/>
+      <c r="J59" s="85" t="s">
         <v>61</v>
       </c>
       <c r="K59" s="34"/>
@@ -7680,16 +7802,16 @@
       <c r="N59" s="48"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="60"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="33"/>
       <c r="C60" s="33"/>
       <c r="D60" s="33"/>
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
       <c r="G60" s="33"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="44"/>
-      <c r="J60" s="83"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="85"/>
       <c r="K60" s="34"/>
       <c r="L60" s="16" t="b">
         <v>1</v>
@@ -7700,57 +7822,57 @@
       <c r="N60" s="48"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="61"/>
-      <c r="B61" s="94" t="s">
+      <c r="A61" s="51"/>
+      <c r="B61" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="94"/>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
-      <c r="F61" s="94"/>
-      <c r="G61" s="94"/>
-      <c r="H61" s="94"/>
-      <c r="I61" s="94"/>
-      <c r="J61" s="94"/>
-      <c r="K61" s="94"/>
-      <c r="L61" s="94"/>
-      <c r="M61" s="94"/>
-      <c r="N61" s="95"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="71"/>
+      <c r="E61" s="71"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="71"/>
+      <c r="L61" s="71"/>
+      <c r="M61" s="71"/>
+      <c r="N61" s="72"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="54" t="s">
+      <c r="B62" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
-      <c r="J62" s="54"/>
-      <c r="K62" s="54"/>
-      <c r="L62" s="54"/>
-      <c r="M62" s="54"/>
-      <c r="N62" s="55"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="46"/>
+      <c r="M62" s="46"/>
+      <c r="N62" s="47"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="68"/>
-      <c r="B63" s="44" t="s">
+      <c r="B63" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="50" t="s">
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F63" s="50"/>
-      <c r="G63" s="50"/>
-      <c r="H63" s="50"/>
-      <c r="I63" s="50"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
       <c r="J63" s="14" t="s">
         <v>66</v>
       </c>
@@ -7763,24 +7885,24 @@
       <c r="M63" s="2">
         <v>5</v>
       </c>
-      <c r="N63" s="93" cm="1">
-        <f t="array" ref="N63">IF(AND(INDEX(Sheet2!A2:A9,Sheet1!K63,1)+INDEX(Sheet2!A2:A9,Sheet1!K64,1)&gt;5,AND(L63,L64)=TRUE),"NA",IF(IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)=0,"",IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)))</f>
+      <c r="N63" s="99" cm="1">
+        <f t="array" ref="N63">IF(AND(AND(L63,L64)=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)+INDEX(Sheet2!A2:A9,Sheet1!K64,1)&gt;5),"NA",IF(AND(K67&gt;K64),"NA",IF(AND(K67=1,K64&gt;2),"NA",IF(IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)=0,"",IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)))))</f>
         <v>140</v>
       </c>
       <c r="O63" s="10"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="68"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
-      <c r="E64" s="50" t="s">
+      <c r="B64" s="73"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F64" s="50"/>
-      <c r="G64" s="50"/>
-      <c r="H64" s="50"/>
-      <c r="I64" s="50"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
       <c r="J64" s="14" t="s">
         <v>67</v>
       </c>
@@ -7793,21 +7915,21 @@
       <c r="M64" s="2">
         <v>10</v>
       </c>
-      <c r="N64" s="48"/>
+      <c r="N64" s="100"/>
       <c r="O64" s="10"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="68"/>
-      <c r="B65" s="44"/>
-      <c r="C65" s="44"/>
-      <c r="D65" s="44"/>
-      <c r="E65" s="50" t="s">
+      <c r="B65" s="73"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="F65" s="50"/>
-      <c r="G65" s="50"/>
-      <c r="H65" s="50"/>
-      <c r="I65" s="50"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
       <c r="J65" s="14" t="s">
         <v>68</v>
       </c>
@@ -7818,20 +7940,20 @@
       <c r="M65" s="2">
         <v>20</v>
       </c>
-      <c r="N65" s="48"/>
+      <c r="N65" s="100"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="68"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
-      <c r="E66" s="50" t="s">
+      <c r="B66" s="73"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="F66" s="50"/>
-      <c r="G66" s="50"/>
-      <c r="H66" s="50"/>
-      <c r="I66" s="50"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
       <c r="J66" s="14" t="s">
         <v>68</v>
       </c>
@@ -7842,81 +7964,82 @@
       <c r="M66" s="2">
         <v>20</v>
       </c>
-      <c r="N66" s="48"/>
+      <c r="N66" s="100"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="58"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="70" t="s">
+      <c r="A67" s="69"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="F67" s="70"/>
-      <c r="G67" s="70"/>
-      <c r="H67" s="70"/>
-      <c r="I67" s="70"/>
+      <c r="F67" s="66"/>
+      <c r="G67" s="66"/>
+      <c r="H67" s="66"/>
+      <c r="I67" s="66"/>
       <c r="J67" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="K67" s="19"/>
-      <c r="L67" s="99" t="b">
-        <f>IF(L64=TRUE,TRUE,FALSE)</f>
+      <c r="K67" s="19">
+        <v>6</v>
+      </c>
+      <c r="L67" s="44" t="b">
         <v>1</v>
       </c>
       <c r="M67" s="2">
         <v>10</v>
       </c>
-      <c r="N67" s="49"/>
+      <c r="N67" s="101"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="59" t="s">
+      <c r="A68" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="84" t="s">
+      <c r="B68" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="C68" s="84"/>
-      <c r="D68" s="84"/>
-      <c r="E68" s="84"/>
-      <c r="F68" s="84"/>
-      <c r="G68" s="84"/>
-      <c r="H68" s="84"/>
-      <c r="I68" s="84"/>
-      <c r="J68" s="84"/>
-      <c r="K68" s="84"/>
-      <c r="L68" s="84"/>
-      <c r="M68" s="84"/>
-      <c r="N68" s="85"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
+      <c r="K68" s="55"/>
+      <c r="L68" s="55"/>
+      <c r="M68" s="55"/>
+      <c r="N68" s="56"/>
       <c r="O68" s="43"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="60"/>
-      <c r="B69" s="50" t="s">
+      <c r="A69" s="50"/>
+      <c r="B69" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="50">
+      <c r="C69" s="45">
         <v>2</v>
       </c>
-      <c r="D69" s="50"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="50"/>
-      <c r="H69" s="50"/>
-      <c r="I69" s="50"/>
-      <c r="J69" s="50"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
       <c r="K69" s="42">
         <v>7</v>
       </c>
       <c r="L69" s="30"/>
       <c r="M69" s="26"/>
-      <c r="N69" s="86" cm="1">
+      <c r="N69" s="57" cm="1">
         <f t="array" ref="N69">INDEX(Sheet2!C2:D8,VALUE(Sheet1!K69),2)</f>
         <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="61"/>
+      <c r="A70" s="51"/>
       <c r="B70" s="35" t="s">
         <v>72</v>
       </c>
@@ -7941,7 +8064,7 @@
       <c r="K70" s="36"/>
       <c r="L70" s="37"/>
       <c r="M70" s="37"/>
-      <c r="N70" s="87"/>
+      <c r="N70" s="58"/>
     </row>
     <row r="71" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="80" t="s">
@@ -7961,10 +8084,10 @@
       <c r="M71" s="82"/>
       <c r="N71" s="15">
         <f>IF(OR(N69="NA",N63="NA",N55="NA",N52="NA",N48="NA",N43="NA",N40="NA",N37="NA",N34="NA",N30="NA",N27="NA",N24="NA",N22="NA",N18="NA",N15="NA",N12="NA",N8="NA",N6="NA"),"NA",SUM(N69,N63,N55,N52,N48,N43,N40,N37,N34,N30,N27,N24,N22,N18,N15,N12,N8,N6))</f>
-        <v>720</v>
+        <v>740</v>
       </c>
       <c r="O71" s="38" t="str">
-        <f>IF(N71=720,"🌟","")</f>
+        <f>IF(N71=740,"🌟","")</f>
         <v>🌟</v>
       </c>
     </row>
@@ -7975,18 +8098,85 @@
       <c r="K77" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="116">
-    <mergeCell ref="E66:I66"/>
-    <mergeCell ref="B51:N51"/>
-    <mergeCell ref="N55:N60"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B42:N42"/>
-    <mergeCell ref="B50:J50"/>
-    <mergeCell ref="B69:J69"/>
-    <mergeCell ref="B68:N68"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="N69:N70"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="B12:E13"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B33:N33"/>
+    <mergeCell ref="B39:N39"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B8:E10"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="B24:G25"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="A71:M71"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="N48:N50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="B52:H53"/>
+    <mergeCell ref="I52:J53"/>
+    <mergeCell ref="H55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="H57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="B54:N54"/>
+    <mergeCell ref="B47:N47"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
     <mergeCell ref="L1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
@@ -8011,313 +8201,269 @@
     <mergeCell ref="B37:J38"/>
     <mergeCell ref="M37:M38"/>
     <mergeCell ref="N37:N38"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="A71:M71"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="N48:N50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="B52:H53"/>
-    <mergeCell ref="I52:J53"/>
-    <mergeCell ref="H55:I56"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="H59:I60"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="B54:N54"/>
-    <mergeCell ref="B47:N47"/>
-    <mergeCell ref="B48:J48"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="E66:I66"/>
+    <mergeCell ref="B51:N51"/>
+    <mergeCell ref="N55:N60"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B42:N42"/>
+    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="B69:J69"/>
+    <mergeCell ref="B68:N68"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="N69:N70"/>
     <mergeCell ref="N43:N46"/>
     <mergeCell ref="B43:H44"/>
     <mergeCell ref="B45:H46"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:N14"/>
-    <mergeCell ref="B11:N11"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B8:E10"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="B24:G25"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="B21:N21"/>
     <mergeCell ref="B40:H41"/>
     <mergeCell ref="N40:N41"/>
-    <mergeCell ref="N18:N20"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="B12:E13"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="B33:N33"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="N34:N35"/>
   </mergeCells>
   <conditionalFormatting sqref="N12:N13">
-    <cfRule type="expression" dxfId="61" priority="65">
+    <cfRule type="expression" dxfId="66" priority="71">
       <formula>$N$12=30</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="66">
+    <cfRule type="expression" dxfId="65" priority="72">
       <formula>$N$12=20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="67">
+    <cfRule type="expression" dxfId="64" priority="73">
       <formula>$N$12="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6">
-    <cfRule type="expression" dxfId="58" priority="64">
+    <cfRule type="expression" dxfId="63" priority="70">
       <formula>$N$6=$M$6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:N10">
-    <cfRule type="expression" dxfId="57" priority="63">
+    <cfRule type="expression" dxfId="62" priority="69">
       <formula>$N$8=$M$8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:N16">
-    <cfRule type="expression" dxfId="56" priority="57">
+    <cfRule type="expression" dxfId="61" priority="63">
       <formula>$N$15=$M$15+$M$16</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="58">
+    <cfRule type="expression" dxfId="60" priority="64">
       <formula>$N$15&lt;30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N18:N20">
-    <cfRule type="expression" dxfId="54" priority="50">
+    <cfRule type="expression" dxfId="59" priority="56">
       <formula>$N$18=$M$20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="51">
+    <cfRule type="expression" dxfId="58" priority="57">
       <formula>$N$18=$M$19</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="52">
+    <cfRule type="expression" dxfId="57" priority="58">
       <formula>$N$18=$M$18</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="53">
+    <cfRule type="expression" dxfId="56" priority="59">
       <formula>$N$18=$M$18+$M$20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="54">
+    <cfRule type="expression" dxfId="55" priority="60">
       <formula>$N$18=$M$19+$M$20</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="55">
+    <cfRule type="expression" dxfId="54" priority="61">
       <formula>$N$18=$M$18+$M$19</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="56">
+    <cfRule type="expression" dxfId="53" priority="62">
       <formula>$N$18=$M$18+$M$19+$M$20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N22">
-    <cfRule type="expression" dxfId="47" priority="49">
+    <cfRule type="expression" dxfId="52" priority="55">
       <formula>$N$22=$M$22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24:N25">
-    <cfRule type="expression" dxfId="46" priority="46">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>N24=M25</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="47">
+    <cfRule type="expression" dxfId="50" priority="53">
       <formula>N24=M24</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="48">
+    <cfRule type="expression" dxfId="49" priority="54">
       <formula>N24="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27:N28">
-    <cfRule type="expression" dxfId="43" priority="43">
+    <cfRule type="expression" dxfId="48" priority="49">
       <formula>N27&lt;30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:N32">
-    <cfRule type="expression" dxfId="42" priority="36">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>N30=M30</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="37">
+    <cfRule type="expression" dxfId="46" priority="43">
       <formula>N30=M31</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="45" priority="44">
       <formula>N30=M32</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="39">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>N30=M30+M31</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="40">
+    <cfRule type="expression" dxfId="43" priority="46">
       <formula>N30=M31+M32</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="41">
+    <cfRule type="expression" dxfId="42" priority="47">
       <formula>N30=M30+M32</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="42">
+    <cfRule type="expression" dxfId="41" priority="48">
       <formula>N30=M30+M31+M32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34:N35">
-    <cfRule type="expression" dxfId="35" priority="33">
+    <cfRule type="expression" dxfId="40" priority="39">
       <formula>N34=M34</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="34">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>N34=M35</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="35">
+    <cfRule type="expression" dxfId="38" priority="41">
       <formula>N34=M34+M35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37">
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>N37=M37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:N41">
-    <cfRule type="expression" dxfId="31" priority="29">
+    <cfRule type="expression" dxfId="36" priority="35">
       <formula>N40=M41</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>N40=M40</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="31">
+    <cfRule type="expression" dxfId="34" priority="37">
       <formula>N40="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43:N46">
-    <cfRule type="expression" dxfId="28" priority="21">
+    <cfRule type="expression" dxfId="33" priority="27">
       <formula>N43=M44+M46</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="22">
+    <cfRule type="expression" dxfId="32" priority="28">
       <formula>N43=M44+M45</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="23">
+    <cfRule type="expression" dxfId="31" priority="29">
       <formula>N43=M44</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="24">
+    <cfRule type="expression" dxfId="30" priority="30">
       <formula>N43=M43+M45</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>N43=M43</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="26">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>N43=M46</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="27">
+    <cfRule type="expression" dxfId="27" priority="33">
       <formula>N43=M45</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="28">
+    <cfRule type="expression" dxfId="26" priority="34">
       <formula>N43="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48:N50">
-    <cfRule type="expression" dxfId="20" priority="14">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>N48=M48</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="24" priority="21">
       <formula>N48=M49</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="16">
+    <cfRule type="expression" dxfId="23" priority="22">
       <formula>N48=M50</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="17">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>N48=M48+M50</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>N48=M49+M50</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="20" priority="25">
       <formula>N48=M48+M49</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="20">
+    <cfRule type="expression" dxfId="19" priority="26">
       <formula>N48=M48+M49+M50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N52:N53">
-    <cfRule type="expression" dxfId="13" priority="11">
+    <cfRule type="expression" dxfId="18" priority="17">
       <formula>N52=M52</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>N52=M53</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="16" priority="19">
       <formula>N52=M52+M53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N55:N60">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>AND(N55&lt;120, N55&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>N55=SUM(M55:M60)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N63:N67">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>AND(0&lt;N63,N63&lt;140)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>N63=140</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$N$63="NA"</formula>
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="NA">
+      <formula>NOT(ISERROR(SEARCH("NA",N63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N2">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>N1&lt;775</formula>
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>N1&lt;740</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>N1=775</formula>
+    <cfRule type="expression" dxfId="1" priority="12">
+      <formula>740</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>$N$1="NA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N69:N70">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>N69&lt;50</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>$N$69=50</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="expression" dxfId="3" priority="44">
+    <cfRule type="expression" dxfId="7" priority="50">
       <formula>N27=M27+M28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
+      <formula>$K$64</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>IF($K$64&gt;1,$K$67&lt;2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L67">
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>$K$67&gt;$K$64</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L64">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
+      <formula>$L$67</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N71">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>740</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9317,6 +9463,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1101" r:id="rId48" name="Drop Down 77">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
+                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:row>66</xdr:row>
+                    <xdr:rowOff>12700</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>11</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>66</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
@@ -9329,18 +9497,22 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>102</v>
       </c>
+      <c r="B1" s="41" t="s">
+        <v>106</v>
+      </c>
       <c r="C1" s="98" t="s">
         <v>103</v>
       </c>
@@ -9350,7 +9522,9 @@
       <c r="A2" s="40">
         <v>0</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
       <c r="C2">
         <v>0</v>
       </c>
@@ -9362,7 +9536,9 @@
       <c r="A3" s="40">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
       <c r="C3">
         <v>1</v>
       </c>
@@ -9374,7 +9550,9 @@
       <c r="A4" s="40">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
       <c r="C4">
         <v>2</v>
       </c>
@@ -9386,7 +9564,9 @@
       <c r="A5" s="40">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
       <c r="C5">
         <v>3</v>
       </c>
@@ -9398,7 +9578,9 @@
       <c r="A6" s="40">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="9">
+        <v>4</v>
+      </c>
       <c r="C6">
         <v>4</v>
       </c>
@@ -9410,7 +9592,9 @@
       <c r="A7" s="40">
         <v>5</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="9">
+        <v>5</v>
+      </c>
       <c r="C7">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
final correction to conditional formatting and calculation constraint for cargo connect.
</commit_message>
<xml_diff>
--- a/Score Sheet/Rocking_Rover-Score_Sheet.xlsx
+++ b/Score Sheet/Rocking_Rover-Score_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdongol/RockingRover/Score Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2334DE-0CA0-6A40-9F18-99E4F20445EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A4053F-0AEE-034B-AF78-81D9BCB9D1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{5677EDF9-9A5E-3B4C-B208-F3D76B1A2241}"/>
   </bookViews>
@@ -913,24 +913,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -939,17 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -961,59 +934,98 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1035,53 +1047,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6466,8 +6466,8 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="95" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:E13"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6487,27 +6487,27 @@
       <c r="A1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="85" t="s">
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="85"/>
-      <c r="N1" s="86">
+      <c r="M1" s="64"/>
+      <c r="N1" s="65">
         <f>IF(OR(N69="NA",N63="NA",N55="NA",N52="NA",N48="NA",N43="NA",N40="NA",N37="NA",N34="NA",N30="NA",N27="NA",N24="NA",N22="NA",N18="NA",N15="NA",N12="NA",N8="NA",N6="NA"),"NA",SUM(N69,N63,N55,N52,N48,N43,N40,N37,N34,N30,N27,N24,N22,N18,N15,N12,N8,N6))</f>
         <v>740</v>
       </c>
-      <c r="O1" s="87" t="str">
+      <c r="O1" s="66" t="str">
         <f>IF(N1=740,"🌟","")</f>
         <v>🌟</v>
       </c>
@@ -6516,22 +6516,22 @@
       <c r="A2" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="89">
+      <c r="B2" s="70">
         <v>52520</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="87"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="66"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
@@ -6551,61 +6551,61 @@
       <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:15" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="88"/>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-      <c r="J4" s="88"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="63" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="64"/>
+      <c r="M4" s="69"/>
       <c r="N4" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O4" s="23"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="47"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="57"/>
-      <c r="B6" s="55" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="93" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
       <c r="K6" s="25"/>
       <c r="L6" s="12" t="b">
         <v>1</v>
@@ -6619,123 +6619,123 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="52"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="47"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="59"/>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="49" t="s">
+      <c r="G8" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="45" t="b">
+      <c r="L8" s="99" t="b">
         <v>1</v>
       </c>
-      <c r="M8" s="65">
+      <c r="M8" s="81">
         <v>20</v>
       </c>
-      <c r="N8" s="53">
+      <c r="N8" s="62">
         <f>IF(L8=TRUE,M8,"")</f>
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="53"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="62"/>
     </row>
     <row r="10" spans="1:15" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="60"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="95"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
       <c r="K10" s="27"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="54"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="63"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="46" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="52"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="47"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="67"/>
-      <c r="B12" s="47" t="s">
+      <c r="A12" s="73"/>
+      <c r="B12" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="47"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="23"/>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
       <c r="K12" s="26"/>
       <c r="L12" s="16" t="b">
         <v>0</v>
@@ -6743,24 +6743,24 @@
       <c r="M12" s="2">
         <v>20</v>
       </c>
-      <c r="N12" s="53">
+      <c r="N12" s="62">
         <f>IF(AND(L12,L13)=TRUE,"NA",IF(L12=TRUE,M12,IF(L13=TRUE,M13,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="57"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
       <c r="F13" s="23"/>
-      <c r="G13" s="50" t="s">
+      <c r="G13" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="54"/>
       <c r="K13" s="26"/>
       <c r="L13" s="16" t="b">
         <v>1</v>
@@ -6768,41 +6768,41 @@
       <c r="M13" s="3">
         <v>30</v>
       </c>
-      <c r="N13" s="54"/>
+      <c r="N13" s="63"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="78"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="91"/>
+      <c r="F14" s="91"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
+      <c r="J14" s="91"/>
+      <c r="K14" s="91"/>
+      <c r="L14" s="91"/>
+      <c r="M14" s="91"/>
+      <c r="N14" s="92"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="59"/>
-      <c r="B15" s="75" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="90"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
       <c r="K15" s="28"/>
       <c r="L15" s="16" t="b">
         <v>1</v>
@@ -6810,24 +6810,24 @@
       <c r="M15" s="2">
         <v>20</v>
       </c>
-      <c r="N15" s="53">
+      <c r="N15" s="62">
         <f>IF(AND(L15,L16)=TRUE,M15+M16,IF(L15=TRUE,M15,IF(L16=TRUE,M16,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="60"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="54"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
       <c r="K16" s="26"/>
       <c r="L16" s="16" t="b">
         <v>1</v>
@@ -6835,41 +6835,41 @@
       <c r="M16" s="3">
         <v>10</v>
       </c>
-      <c r="N16" s="54"/>
+      <c r="N16" s="63"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="52"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="47"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="67"/>
-      <c r="B18" s="70" t="s">
+      <c r="A18" s="73"/>
+      <c r="B18" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
       <c r="K18" s="29"/>
       <c r="L18" s="16" t="b">
         <v>1</v>
@@ -6877,24 +6877,24 @@
       <c r="M18" s="2">
         <v>10</v>
       </c>
-      <c r="N18" s="73">
+      <c r="N18" s="48">
         <f>IF(AND(L18,L19,L20)=TRUE,M18+M19+M20,IF(AND(L18,L19)=TRUE,M18+M19,IF(AND(L19,L20)=TRUE,M19+M20,IF(AND(L18,L20)=TRUE,M18+M20,IF(L18=TRUE,M18,IF(L19=TRUE,M19,IF(L20=TRUE,M20,"")))))))</f>
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="67"/>
-      <c r="B19" s="49" t="s">
+      <c r="A19" s="73"/>
+      <c r="B19" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
       <c r="K19" s="26"/>
       <c r="L19" s="16" t="b">
         <v>1</v>
@@ -6902,21 +6902,21 @@
       <c r="M19" s="2">
         <v>10</v>
       </c>
-      <c r="N19" s="73"/>
+      <c r="N19" s="48"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="57"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="74"/>
+      <c r="B20" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
       <c r="K20" s="26"/>
       <c r="L20" s="16" t="b">
         <v>1</v>
@@ -6924,41 +6924,41 @@
       <c r="M20" s="3">
         <v>10</v>
       </c>
-      <c r="N20" s="74"/>
+      <c r="N20" s="59"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="52"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="60"/>
-      <c r="B22" s="72" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="98"/>
       <c r="K22" s="4"/>
       <c r="L22" s="16" t="b">
         <v>1</v>
@@ -6972,35 +6972,35 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="52"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="47"/>
     </row>
     <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="67"/>
-      <c r="B24" s="68" t="s">
+      <c r="A24" s="73"/>
+      <c r="B24" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
       <c r="H24" s="23"/>
       <c r="I24" s="30" t="s">
         <v>86</v>
@@ -7013,19 +7013,19 @@
       <c r="M24" s="2">
         <v>20</v>
       </c>
-      <c r="N24" s="53">
+      <c r="N24" s="62">
         <f>IF(AND(L24,L25)=TRUE,"NA",IF(L24=TRUE,M24,IF(L25=TRUE,M25,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="57"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
+      <c r="A25" s="74"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
       <c r="H25" s="23"/>
       <c r="I25" s="25" t="s">
         <v>87</v>
@@ -7038,41 +7038,41 @@
       <c r="M25" s="3">
         <v>30</v>
       </c>
-      <c r="N25" s="54"/>
+      <c r="N25" s="63"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="52"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="59"/>
-      <c r="B27" s="49" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="45"/>
       <c r="K27" s="26"/>
       <c r="L27" s="16" t="b">
         <v>1</v>
@@ -7080,24 +7080,24 @@
       <c r="M27" s="6">
         <v>20</v>
       </c>
-      <c r="N27" s="53">
+      <c r="N27" s="62">
         <f>IF(IF(L27=TRUE,M27,0)+IF(L28=TRUE,M28,0)=0, "", IF(L27=TRUE,M27,0)+IF(L28=TRUE,M28,0))</f>
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="60"/>
-      <c r="B28" s="50" t="s">
+      <c r="A28" s="51"/>
+      <c r="B28" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
       <c r="K28" s="26"/>
       <c r="L28" s="16" t="b">
         <v>1</v>
@@ -7105,41 +7105,41 @@
       <c r="M28" s="7">
         <v>10</v>
       </c>
-      <c r="N28" s="54"/>
+      <c r="N28" s="63"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="52"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="47"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="67"/>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="73"/>
+      <c r="B30" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
       <c r="K30" s="26"/>
       <c r="L30" s="16" t="b">
         <v>1</v>
@@ -7147,24 +7147,24 @@
       <c r="M30" s="6">
         <v>20</v>
       </c>
-      <c r="N30" s="73">
+      <c r="N30" s="48">
         <f>IF(AND(L30,L31,L32)=TRUE,M30+M31+M32,IF(AND(L30,L31)=TRUE,M30+M31,IF(AND(L31,L32)=TRUE,M31+M32,IF(AND(L30,L32)=TRUE,M30+M32,IF(L30=TRUE,M30,IF(L31=TRUE,M31,IF(L32=TRUE,M32,"")))))))</f>
         <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="67"/>
-      <c r="B31" s="49" t="s">
+      <c r="A31" s="73"/>
+      <c r="B31" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
       <c r="K31" s="26"/>
       <c r="L31" s="16" t="b">
         <v>1</v>
@@ -7172,21 +7172,21 @@
       <c r="M31" s="6">
         <v>10</v>
       </c>
-      <c r="N31" s="73"/>
+      <c r="N31" s="48"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="57"/>
-      <c r="B32" s="50" t="s">
+      <c r="A32" s="74"/>
+      <c r="B32" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
       <c r="K32" s="26"/>
       <c r="L32" s="16" t="b">
         <v>1</v>
@@ -7194,41 +7194,41 @@
       <c r="M32" s="7">
         <v>10</v>
       </c>
-      <c r="N32" s="74"/>
+      <c r="N32" s="59"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="58" t="s">
+      <c r="A33" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="52"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="47"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="59"/>
-      <c r="B34" s="49" t="s">
+      <c r="A34" s="50"/>
+      <c r="B34" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
+      <c r="C34" s="45"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
       <c r="K34" s="26"/>
       <c r="L34" s="16" t="b">
         <v>1</v>
@@ -7236,24 +7236,24 @@
       <c r="M34" s="6">
         <v>20</v>
       </c>
-      <c r="N34" s="53">
+      <c r="N34" s="62">
         <f>IF(AND(L34,L35)=TRUE,M34+M35,IF(L34=TRUE,M34,IF(L35=TRUE,M35,"")))</f>
         <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="60"/>
-      <c r="B35" s="50" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="54" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
       <c r="K35" s="26"/>
       <c r="L35" s="16" t="b">
         <v>1</v>
@@ -7261,104 +7261,104 @@
       <c r="M35" s="7">
         <v>20</v>
       </c>
-      <c r="N35" s="54"/>
+      <c r="N35" s="63"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="51"/>
-      <c r="I36" s="51"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
-      <c r="N36" s="52"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="47"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="67"/>
-      <c r="B37" s="68" t="s">
+      <c r="A37" s="73"/>
+      <c r="B37" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="80"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
       <c r="K37" s="31"/>
-      <c r="L37" s="79" t="b">
+      <c r="L37" s="83" t="b">
         <v>1</v>
       </c>
-      <c r="M37" s="65">
+      <c r="M37" s="81">
         <v>20</v>
       </c>
-      <c r="N37" s="73">
+      <c r="N37" s="48">
         <f t="shared" ref="N37" si="0">IF(L37=TRUE,M37,"")</f>
         <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="57"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
-      <c r="G38" s="69"/>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
-      <c r="J38" s="69"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71"/>
+      <c r="I38" s="71"/>
+      <c r="J38" s="71"/>
       <c r="K38" s="32"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="66"/>
-      <c r="N38" s="74"/>
+      <c r="L38" s="84"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="59"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="58" t="s">
+      <c r="A39" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51"/>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="52"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="47"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="59"/>
-      <c r="B40" s="47" t="s">
+      <c r="A40" s="50"/>
+      <c r="B40" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="47"/>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-      <c r="I40" s="49" t="s">
+      <c r="C40" s="60"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
+      <c r="I40" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="J40" s="49"/>
+      <c r="J40" s="45"/>
       <c r="K40" s="26"/>
       <c r="L40" s="16" t="b">
         <v>0</v>
@@ -7366,24 +7366,24 @@
       <c r="M40" s="2">
         <v>20</v>
       </c>
-      <c r="N40" s="53">
+      <c r="N40" s="62">
         <f>IF(AND(L40,L41)=TRUE,"NA",IF(L40=TRUE,M40,IF(L41=TRUE,M41,"")))</f>
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="60"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="50" t="s">
+      <c r="A41" s="51"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="J41" s="50"/>
+      <c r="J41" s="54"/>
       <c r="K41" s="26"/>
       <c r="L41" s="16" t="b">
         <v>1</v>
@@ -7391,43 +7391,43 @@
       <c r="M41" s="3">
         <v>30</v>
       </c>
-      <c r="N41" s="54"/>
+      <c r="N41" s="63"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="95"/>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="95"/>
-      <c r="L42" s="95"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="96"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="53"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="67"/>
-      <c r="B43" s="47" t="s">
+      <c r="A43" s="73"/>
+      <c r="B43" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="49" t="s">
+      <c r="C43" s="60"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="60"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="J43" s="49"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="26"/>
       <c r="L43" s="16" t="b">
         <v>0</v>
@@ -7435,24 +7435,24 @@
       <c r="M43" s="2">
         <v>20</v>
       </c>
-      <c r="N43" s="73">
+      <c r="N43" s="48">
         <f>IF(AND(L43,L44,L45,L46)=TRUE,"NA",IF(AND(L43,L44)=TRUE,"NA",IF(AND(L45,L46)=TRUE,"NA",IF(AND(L43,L45)=TRUE,M43+M45,IF(AND(L43,L46)=TRUE,M43+M46,IF(AND(L44,L45)=TRUE,M44+M45,IF(AND(L44,L46)=TRUE,M44+M46,IF(L43=TRUE,M43,IF(L44=TRUE,M44,IF(L45=TRUE,M45,IF(L46=TRUE,M46,"")))))))))))</f>
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="67"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="49" t="s">
+      <c r="A44" s="73"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="60"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="J44" s="49"/>
+      <c r="J44" s="45"/>
       <c r="K44" s="26"/>
       <c r="L44" s="16" t="b">
         <v>1</v>
@@ -7460,23 +7460,23 @@
       <c r="M44" s="2">
         <v>30</v>
       </c>
-      <c r="N44" s="73"/>
+      <c r="N44" s="48"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="67"/>
-      <c r="B45" s="47" t="s">
+      <c r="A45" s="73"/>
+      <c r="B45" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="47"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="49" t="s">
+      <c r="C45" s="60"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="60"/>
+      <c r="I45" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="J45" s="49"/>
+      <c r="J45" s="45"/>
       <c r="K45" s="26"/>
       <c r="L45" s="16" t="b">
         <v>0</v>
@@ -7484,21 +7484,21 @@
       <c r="M45" s="2">
         <v>5</v>
       </c>
-      <c r="N45" s="73"/>
+      <c r="N45" s="48"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="57"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="50" t="s">
+      <c r="A46" s="74"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="J46" s="50"/>
+      <c r="J46" s="54"/>
       <c r="K46" s="26"/>
       <c r="L46" s="16" t="b">
         <v>1</v>
@@ -7506,41 +7506,41 @@
       <c r="M46" s="3">
         <v>10</v>
       </c>
-      <c r="N46" s="74"/>
+      <c r="N46" s="59"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="58" t="s">
+      <c r="A47" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C47" s="51"/>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="51"/>
-      <c r="I47" s="51"/>
-      <c r="J47" s="51"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="52"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="46"/>
+      <c r="N47" s="47"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="59"/>
-      <c r="B48" s="49" t="s">
+      <c r="A48" s="50"/>
+      <c r="B48" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="49"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
       <c r="K48" s="26"/>
       <c r="L48" s="16" t="b">
         <v>1</v>
@@ -7548,24 +7548,24 @@
       <c r="M48" s="2">
         <v>10</v>
       </c>
-      <c r="N48" s="73">
+      <c r="N48" s="48">
         <f>IF(AND(L48,L49,L50)=TRUE,M48+M49+M50,IF(AND(L48,L49)=TRUE,M48+M49,IF(AND(L49,L50)=TRUE,M49+M50,IF(AND(L48,L50)=TRUE,M48+M50,IF(L48=TRUE,M48,IF(L49=TRUE,M49,IF(L50=TRUE,M50,"")))))))</f>
         <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A49" s="59"/>
-      <c r="B49" s="49" t="s">
+      <c r="A49" s="50"/>
+      <c r="B49" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
       <c r="K49" s="26"/>
       <c r="L49" s="16" t="b">
         <v>1</v>
@@ -7573,21 +7573,21 @@
       <c r="M49" s="2">
         <v>10</v>
       </c>
-      <c r="N49" s="73"/>
+      <c r="N49" s="48"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A50" s="60"/>
-      <c r="B50" s="50" t="s">
+      <c r="A50" s="51"/>
+      <c r="B50" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
       <c r="K50" s="26"/>
       <c r="L50" s="16" t="b">
         <v>1</v>
@@ -7595,43 +7595,43 @@
       <c r="M50" s="3">
         <v>10</v>
       </c>
-      <c r="N50" s="74"/>
+      <c r="N50" s="59"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A51" s="56" t="s">
+      <c r="A51" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="51" t="s">
+      <c r="B51" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="51"/>
-      <c r="I51" s="51"/>
-      <c r="J51" s="51"/>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
-      <c r="M51" s="51"/>
-      <c r="N51" s="52"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="47"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A52" s="67"/>
-      <c r="B52" s="47" t="s">
+      <c r="A52" s="73"/>
+      <c r="B52" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47" t="s">
+      <c r="C52" s="60"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="60"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+      <c r="H52" s="60"/>
+      <c r="I52" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="J52" s="47"/>
+      <c r="J52" s="60"/>
       <c r="K52" s="33"/>
       <c r="L52" s="16" t="b">
         <v>1</v>
@@ -7639,22 +7639,22 @@
       <c r="M52" s="2">
         <v>10</v>
       </c>
-      <c r="N52" s="53">
+      <c r="N52" s="62">
         <f>IF(AND(L52,L53)=TRUE,M52+M53,IF(L52=TRUE,M52,IF(L53=TRUE,M53,"")))</f>
         <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A53" s="57"/>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
-      <c r="J53" s="48"/>
+      <c r="A53" s="74"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="61"/>
+      <c r="I53" s="61"/>
+      <c r="J53" s="61"/>
       <c r="K53" s="33"/>
       <c r="L53" s="16" t="b">
         <v>1</v>
@@ -7662,43 +7662,43 @@
       <c r="M53" s="2">
         <v>10</v>
       </c>
-      <c r="N53" s="54"/>
+      <c r="N53" s="63"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" s="58" t="s">
+      <c r="A54" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="51"/>
-      <c r="I54" s="51"/>
-      <c r="J54" s="51"/>
-      <c r="K54" s="51"/>
-      <c r="L54" s="51"/>
-      <c r="M54" s="51"/>
-      <c r="N54" s="52"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="46"/>
+      <c r="N54" s="47"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="59"/>
-      <c r="B55" s="47" t="s">
+      <c r="A55" s="50"/>
+      <c r="B55" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
-      <c r="H55" s="47" t="s">
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="60"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I55" s="47"/>
-      <c r="J55" s="84" t="s">
+      <c r="I55" s="60"/>
+      <c r="J55" s="88" t="s">
         <v>55</v>
       </c>
       <c r="K55" s="34"/>
@@ -7708,22 +7708,22 @@
       <c r="M55" s="2">
         <v>10</v>
       </c>
-      <c r="N55" s="73">
+      <c r="N55" s="48">
         <f>IF(IF(L55=TRUE,M55,0)+IF(L56=TRUE,M56,0)+IF(L57=TRUE,M57,0)+IF(L58=TRUE,M58,0)+IF(L59=TRUE,M59,0)+IF(L60=TRUE,M60,0)=0,"",                                                                                                  IF(L55=TRUE,M55,0)+IF(L56=TRUE,M56,0)+IF(L57=TRUE,M57,0)+IF(L58=TRUE,M58,0)+IF(L59=TRUE,M59,0)+IF(L60=TRUE,M60,0))</f>
         <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="59"/>
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="84"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="60"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="60"/>
+      <c r="H56" s="60"/>
+      <c r="I56" s="60"/>
+      <c r="J56" s="88"/>
       <c r="K56" s="34"/>
       <c r="L56" s="17" t="b">
         <v>1</v>
@@ -7731,21 +7731,21 @@
       <c r="M56" s="2">
         <v>10</v>
       </c>
-      <c r="N56" s="73"/>
+      <c r="N56" s="48"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="59"/>
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47" t="s">
+      <c r="A57" s="50"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="60"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="60"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="I57" s="47"/>
-      <c r="J57" s="84" t="s">
+      <c r="I57" s="60"/>
+      <c r="J57" s="88" t="s">
         <v>59</v>
       </c>
       <c r="K57" s="34"/>
@@ -7755,19 +7755,19 @@
       <c r="M57" s="2">
         <v>20</v>
       </c>
-      <c r="N57" s="73"/>
+      <c r="N57" s="48"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="59"/>
-      <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-      <c r="J58" s="84"/>
+      <c r="A58" s="50"/>
+      <c r="B58" s="60"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="60"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="88"/>
       <c r="K58" s="34"/>
       <c r="L58" s="16" t="b">
         <v>1</v>
@@ -7775,21 +7775,21 @@
       <c r="M58" s="2">
         <v>20</v>
       </c>
-      <c r="N58" s="73"/>
+      <c r="N58" s="48"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="59"/>
-      <c r="B59" s="47"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47" t="s">
+      <c r="A59" s="50"/>
+      <c r="B59" s="60"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="60"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="60" t="s">
         <v>94</v>
       </c>
-      <c r="I59" s="47"/>
-      <c r="J59" s="84" t="s">
+      <c r="I59" s="60"/>
+      <c r="J59" s="88" t="s">
         <v>60</v>
       </c>
       <c r="K59" s="34"/>
@@ -7799,19 +7799,19 @@
       <c r="M59" s="2">
         <v>30</v>
       </c>
-      <c r="N59" s="73"/>
+      <c r="N59" s="48"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A60" s="59"/>
+      <c r="A60" s="50"/>
       <c r="B60" s="33"/>
       <c r="C60" s="33"/>
       <c r="D60" s="33"/>
       <c r="E60" s="33"/>
       <c r="F60" s="33"/>
       <c r="G60" s="33"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="84"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="88"/>
       <c r="K60" s="34"/>
       <c r="L60" s="16" t="b">
         <v>1</v>
@@ -7819,60 +7819,60 @@
       <c r="M60" s="2">
         <v>30</v>
       </c>
-      <c r="N60" s="73"/>
+      <c r="N60" s="48"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A61" s="60"/>
-      <c r="B61" s="93" t="s">
+      <c r="A61" s="51"/>
+      <c r="B61" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="93"/>
-      <c r="D61" s="93"/>
-      <c r="E61" s="93"/>
-      <c r="F61" s="93"/>
-      <c r="G61" s="93"/>
-      <c r="H61" s="93"/>
-      <c r="I61" s="93"/>
-      <c r="J61" s="93"/>
-      <c r="K61" s="93"/>
-      <c r="L61" s="93"/>
-      <c r="M61" s="93"/>
-      <c r="N61" s="94"/>
+      <c r="C61" s="78"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="78"/>
+      <c r="F61" s="78"/>
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="78"/>
+      <c r="J61" s="78"/>
+      <c r="K61" s="78"/>
+      <c r="L61" s="78"/>
+      <c r="M61" s="78"/>
+      <c r="N61" s="79"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A62" s="56" t="s">
+      <c r="A62" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="B62" s="51" t="s">
+      <c r="B62" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="51"/>
-      <c r="D62" s="51"/>
-      <c r="E62" s="51"/>
-      <c r="F62" s="51"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="51"/>
-      <c r="K62" s="51"/>
-      <c r="L62" s="51"/>
-      <c r="M62" s="51"/>
-      <c r="N62" s="52"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="46"/>
+      <c r="M62" s="46"/>
+      <c r="N62" s="47"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A63" s="67"/>
-      <c r="B63" s="47" t="s">
+      <c r="A63" s="73"/>
+      <c r="B63" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="49" t="s">
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
       <c r="J63" s="14" t="s">
         <v>65</v>
       </c>
@@ -7885,24 +7885,24 @@
       <c r="M63" s="2">
         <v>5</v>
       </c>
-      <c r="N63" s="90" cm="1">
-        <f t="array" ref="N63">IF(AND(AND(L63,L64)=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)+INDEX(Sheet2!A2:A9,Sheet1!K64,1)&gt;5),"NA",IF(AND(K67&gt;K64),"NA",IF(AND(K67=1,K64&gt;2),"NA",IF(IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)=0,"",IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)))))</f>
+      <c r="N63" s="75" cm="1">
+        <f t="array" ref="N63">IF(AND(AND(L63,L64)=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)+INDEX(Sheet2!A2:A9,Sheet1!K64,1)&gt;5),"NA",IF(AND(K67&gt;K64),"NA",IF(AND(INDEX(Sheet2!$B$2:$B$7,K67,0)=0,INDEX(Sheet2!$A$2:$A$7,K64,0)&gt;0),"NA",IF(AND(INDEX(Sheet2!$B$2:$B$7,K64,0)&gt;0,AND(L64,L67)=FALSE),"NA",IF(IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0)=0,"",IF(L63=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K63,1)*Sheet1!M63,0)+IF(L64=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K64,1)*Sheet1!M64,0)+IF(L67=TRUE,INDEX(Sheet2!A2:A9,Sheet1!K67,1)*Sheet1!M67,0)+IF(L65=TRUE,M65,0)+IF(L66=TRUE,M66,0))))))</f>
         <v>140</v>
       </c>
       <c r="O63" s="10"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A64" s="67"/>
-      <c r="B64" s="47"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="49" t="s">
+      <c r="A64" s="73"/>
+      <c r="B64" s="60"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="49"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="45"/>
+      <c r="I64" s="45"/>
       <c r="J64" s="14" t="s">
         <v>66</v>
       </c>
@@ -7915,21 +7915,21 @@
       <c r="M64" s="2">
         <v>10</v>
       </c>
-      <c r="N64" s="91"/>
+      <c r="N64" s="76"/>
       <c r="O64" s="10"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="67"/>
-      <c r="B65" s="47"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="49" t="s">
+      <c r="A65" s="73"/>
+      <c r="B65" s="60"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="49"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
       <c r="J65" s="14" t="s">
         <v>67</v>
       </c>
@@ -7940,20 +7940,20 @@
       <c r="M65" s="2">
         <v>20</v>
       </c>
-      <c r="N65" s="91"/>
+      <c r="N65" s="76"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="67"/>
-      <c r="B66" s="47"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="49" t="s">
+      <c r="A66" s="73"/>
+      <c r="B66" s="60"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
-      <c r="I66" s="49"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="45"/>
+      <c r="I66" s="45"/>
       <c r="J66" s="14" t="s">
         <v>67</v>
       </c>
@@ -7964,20 +7964,20 @@
       <c r="M66" s="2">
         <v>20</v>
       </c>
-      <c r="N66" s="91"/>
+      <c r="N66" s="76"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="57"/>
-      <c r="B67" s="48"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="69" t="s">
+      <c r="A67" s="74"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="F67" s="69"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="69"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="I67" s="71"/>
       <c r="J67" s="13" t="s">
         <v>104</v>
       </c>
@@ -7990,56 +7990,56 @@
       <c r="M67" s="2">
         <v>10</v>
       </c>
-      <c r="N67" s="92"/>
+      <c r="N67" s="77"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="B68" s="97" t="s">
+      <c r="B68" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="C68" s="97"/>
-      <c r="D68" s="97"/>
-      <c r="E68" s="97"/>
-      <c r="F68" s="97"/>
-      <c r="G68" s="97"/>
-      <c r="H68" s="97"/>
-      <c r="I68" s="97"/>
-      <c r="J68" s="97"/>
-      <c r="K68" s="97"/>
-      <c r="L68" s="97"/>
-      <c r="M68" s="97"/>
-      <c r="N68" s="98"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="55"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="55"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
+      <c r="J68" s="55"/>
+      <c r="K68" s="55"/>
+      <c r="L68" s="55"/>
+      <c r="M68" s="55"/>
+      <c r="N68" s="56"/>
       <c r="O68" s="43"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A69" s="59"/>
-      <c r="B69" s="49" t="s">
+      <c r="A69" s="50"/>
+      <c r="B69" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="49">
+      <c r="C69" s="45">
         <v>2</v>
       </c>
-      <c r="D69" s="49"/>
-      <c r="E69" s="49"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="49"/>
-      <c r="H69" s="49"/>
-      <c r="I69" s="49"/>
-      <c r="J69" s="49"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
+      <c r="J69" s="45"/>
       <c r="K69" s="42">
         <v>7</v>
       </c>
       <c r="L69" s="30"/>
       <c r="M69" s="26"/>
-      <c r="N69" s="99" cm="1">
+      <c r="N69" s="57" cm="1">
         <f t="array" ref="N69">INDEX(Sheet2!C2:D8,VALUE(Sheet1!K69),2)</f>
         <v>50</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A70" s="60"/>
+      <c r="A70" s="51"/>
       <c r="B70" s="35" t="s">
         <v>71</v>
       </c>
@@ -8064,24 +8064,24 @@
       <c r="K70" s="36"/>
       <c r="L70" s="37"/>
       <c r="M70" s="37"/>
-      <c r="N70" s="100"/>
+      <c r="N70" s="58"/>
     </row>
     <row r="71" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="81" t="s">
+      <c r="A71" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="B71" s="82"/>
-      <c r="C71" s="82"/>
-      <c r="D71" s="82"/>
-      <c r="E71" s="82"/>
-      <c r="F71" s="82"/>
-      <c r="G71" s="82"/>
-      <c r="H71" s="82"/>
-      <c r="I71" s="82"/>
-      <c r="J71" s="82"/>
-      <c r="K71" s="82"/>
-      <c r="L71" s="82"/>
-      <c r="M71" s="83"/>
+      <c r="B71" s="86"/>
+      <c r="C71" s="86"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
+      <c r="F71" s="86"/>
+      <c r="G71" s="86"/>
+      <c r="H71" s="86"/>
+      <c r="I71" s="86"/>
+      <c r="J71" s="86"/>
+      <c r="K71" s="86"/>
+      <c r="L71" s="86"/>
+      <c r="M71" s="87"/>
       <c r="N71" s="15">
         <f>IF(OR(N69="NA",N63="NA",N55="NA",N52="NA",N48="NA",N43="NA",N40="NA",N37="NA",N34="NA",N30="NA",N27="NA",N24="NA",N22="NA",N18="NA",N15="NA",N12="NA",N8="NA",N6="NA"),"NA",SUM(N69,N63,N55,N52,N48,N43,N40,N37,N34,N30,N27,N24,N22,N18,N15,N12,N8,N6))</f>
         <v>740</v>
@@ -8098,23 +8098,85 @@
       <c r="K77" s="39"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="116">
-    <mergeCell ref="E66:I66"/>
-    <mergeCell ref="B51:N51"/>
-    <mergeCell ref="N55:N60"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B42:N42"/>
-    <mergeCell ref="B50:J50"/>
-    <mergeCell ref="B69:J69"/>
-    <mergeCell ref="B68:N68"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="N69:N70"/>
-    <mergeCell ref="N43:N46"/>
-    <mergeCell ref="B43:H44"/>
-    <mergeCell ref="B45:H46"/>
-    <mergeCell ref="B40:H41"/>
-    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="B12:E13"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B33:N33"/>
+    <mergeCell ref="B39:N39"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B8:E10"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="M8:M10"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B7:N7"/>
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="N8:N10"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="B24:G25"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="N18:N20"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:N14"/>
+    <mergeCell ref="B11:N11"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B30:J30"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="A71:M71"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="N48:N50"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="B52:H53"/>
+    <mergeCell ref="I52:J53"/>
+    <mergeCell ref="H55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="H57:I58"/>
+    <mergeCell ref="J57:J58"/>
+    <mergeCell ref="H59:I60"/>
+    <mergeCell ref="J59:J60"/>
+    <mergeCell ref="B54:N54"/>
+    <mergeCell ref="B47:N47"/>
+    <mergeCell ref="B48:J48"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
     <mergeCell ref="L1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
@@ -8139,83 +8201,21 @@
     <mergeCell ref="B37:J38"/>
     <mergeCell ref="M37:M38"/>
     <mergeCell ref="N37:N38"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="A71:M71"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="N48:N50"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="B52:H53"/>
-    <mergeCell ref="I52:J53"/>
-    <mergeCell ref="H55:I56"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="H57:I58"/>
-    <mergeCell ref="J57:J58"/>
-    <mergeCell ref="H59:I60"/>
-    <mergeCell ref="J59:J60"/>
-    <mergeCell ref="B54:N54"/>
-    <mergeCell ref="B47:N47"/>
-    <mergeCell ref="B48:J48"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="B16:J16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:N14"/>
-    <mergeCell ref="B11:N11"/>
-    <mergeCell ref="B31:J31"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B8:E10"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="M8:M10"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B7:N7"/>
-    <mergeCell ref="B5:N5"/>
-    <mergeCell ref="N8:N10"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="B24:G25"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="B20:J20"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="B21:N21"/>
-    <mergeCell ref="N18:N20"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="B12:E13"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="B32:J32"/>
-    <mergeCell ref="B33:N33"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="E66:I66"/>
+    <mergeCell ref="B51:N51"/>
+    <mergeCell ref="N55:N60"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B42:N42"/>
+    <mergeCell ref="B50:J50"/>
+    <mergeCell ref="B69:J69"/>
+    <mergeCell ref="B68:N68"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="N69:N70"/>
+    <mergeCell ref="N43:N46"/>
+    <mergeCell ref="B43:H44"/>
+    <mergeCell ref="B45:H46"/>
+    <mergeCell ref="B40:H41"/>
+    <mergeCell ref="N40:N41"/>
   </mergeCells>
   <conditionalFormatting sqref="N12:N13">
     <cfRule type="expression" dxfId="66" priority="71">

</xml_diff>